<commit_message>
FAAS-828 Device customization for android
</commit_message>
<xml_diff>
--- a/src/test/resources/FHEO-Devicedata.xlsx
+++ b/src/test/resources/FHEO-Devicedata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krish\IdeaProjects\formservice-testing\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC14127C-CC22-4B05-9844-69DCF3236014}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41D9DED-1831-47CD-BBDE-12DE1779BDAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="474" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
   <si>
     <t>race</t>
   </si>
@@ -183,9 +183,6 @@
     <t>disaltOtherRelationshipDescription</t>
   </si>
   <si>
-    <t>03-04-2021</t>
-  </si>
-  <si>
     <t>morning</t>
   </si>
   <si>
@@ -214,6 +211,15 @@
   </si>
   <si>
     <t>Updik1</t>
+  </si>
+  <si>
+    <t>discDateWithTimestamp</t>
+  </si>
+  <si>
+    <t>05-12-2021</t>
+  </si>
+  <si>
+    <t>2021-05-12T00:00:00</t>
   </si>
 </sst>
 </file>
@@ -751,7 +757,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -790,6 +796,12 @@
     <xf numFmtId="49" fontId="16" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1153,13 +1165,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AK2"/>
+  <dimension ref="A1:AL2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="AG2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomRight" activeCell="AL2" sqref="AL2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1201,10 +1213,11 @@
     <col min="35" max="35" width="29.5234375" style="16" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="24.15625" style="16" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="17" style="16" bestFit="1" customWidth="1"/>
-    <col min="38" max="16384" width="8.83984375" style="1"/>
+    <col min="38" max="38" width="20.83984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1314,10 +1327,13 @@
         <v>41</v>
       </c>
       <c r="AK1" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
@@ -1340,10 +1356,10 @@
         <v>7</v>
       </c>
       <c r="I2" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>58</v>
       </c>
       <c r="K2" s="8" t="s">
         <v>10</v>
@@ -1352,10 +1368,10 @@
         <v>8009098909</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O2" s="8" t="s">
         <v>23</v>
@@ -1369,20 +1385,20 @@
       <c r="R2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="S2" s="8">
+      <c r="S2" s="20">
         <v>20006</v>
       </c>
       <c r="T2" s="11" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="U2" s="5" t="s">
         <v>27</v>
       </c>
       <c r="V2" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="W2" s="13" t="s">
         <v>59</v>
-      </c>
-      <c r="W2" s="13" t="s">
-        <v>60</v>
       </c>
       <c r="X2" s="13">
         <v>2224568749</v>
@@ -1391,7 +1407,7 @@
         <v>43</v>
       </c>
       <c r="Z2" s="18" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AA2" s="5" t="s">
         <v>44</v>
@@ -1400,12 +1416,12 @@
         <v>45</v>
       </c>
       <c r="AC2" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AD2" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="AE2" s="13">
+      <c r="AE2" s="21">
         <v>20006</v>
       </c>
       <c r="AF2" s="16" t="s">
@@ -1424,7 +1440,10 @@
         <v>8009098908</v>
       </c>
       <c r="AK2" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="AL2" s="11" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>